<commit_message>
cap nhat tinh nang tim kiem
</commit_message>
<xml_diff>
--- a/data/fileexcel/product.xlsx
+++ b/data/fileexcel/product.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Q-Aexcel\data\fileexcel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -16,40 +21,107 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>STT</t>
-  </si>
-  <si>
-    <t>product_name</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>php ebook</t>
-  </si>
-  <si>
-    <t>java ebook</t>
-  </si>
-  <si>
-    <t>laravel 5</t>
-  </si>
-  <si>
-    <t>angularjs</t>
-  </si>
-  <si>
-    <t>python</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Function area</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>Doc Version</t>
+  </si>
+  <si>
+    <t>Section/screen</t>
+  </si>
+  <si>
+    <t>Comment/Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Raised by</t>
+  </si>
+  <si>
+    <t>Date raised</t>
+  </si>
+  <si>
+    <t>Pic Answer</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Closed In Version</t>
+  </si>
+  <si>
+    <t>Required finish date</t>
+  </si>
+  <si>
+    <t>Date closed</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ATCB_Bài 1_Phần đọc file</t>
+  </si>
+  <si>
+    <t>Theo như em tìm hiểu trên trang http://www.cplusplus.com/forum/beginner/32200/ thì đoạn code dưới đây dùng để viết vào file trong class Employee:
+int main()
+{  
+   Employee employee1;
+   create_new_employee(employee1);
+   string filename = "employee_test.txt";
+   ofstream outfile;
+   outfile.open (filename.c_str(), ios::out|ios::binary|ios::app);
+   outfile.write ( (char *)(&amp;employee1), sizeof(Employee) );
+   outfile.close();
+   system("pause");
+   return 0;
+}
+Nhưng e k có hiểu chỗ (char *)(&amp;employee1) có nghĩa là gì, và nó in ra những gì,e viết một đoạn code nhỏ để cho in ra kết quả nhưng vẫn chưa có hiểu, mong anh/bạn giải đáp giùm. Thanks all !^^</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>PhungNQ</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>dsaujsadhkjhjkdhkjajd</t>
+  </si>
+  <si>
+    <t>17/10/2017</t>
+  </si>
+  <si>
+    <t>ATCB_Bài 1_Phần đọc file hgbashsahdkjhasjk</t>
+  </si>
+  <si>
+    <t>KhuongNHQ</t>
+  </si>
+  <si>
+    <t>LinhKA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,16 +129,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -74,21 +170,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -137,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -172,7 +338,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -381,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,89 +558,139 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="8"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>50</v>
-      </c>
+    <row r="3" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="8"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>60</v>
-      </c>
+    <row r="4" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>